<commit_message>
Able to get all train stations in a radius and their respective CTA station ids
just need to get which station would get you from point a to point b the fastest and return what time you would need to get to the station by
</commit_message>
<xml_diff>
--- a/CTA train addresses.xlsx
+++ b/CTA train addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59b2effe41531a4b/Documents/GitHub/T.A.U.I-Train-And-Uber-Integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_5E6DB5835B20DB1377192011595ED87656CDF5FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CED8511F-8F13-42D6-8203-26B29A8A2C72}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_5E6DB5835B20DB1377192011595ED87656CDF5FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{755E7143-8651-4EEC-9144-DE6B8384AD50}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="166">
   <si>
     <t>18th</t>
   </si>
   <si>
-    <t>googlemaps</t>
-  </si>
-  <si>
     <t>35th-Bronzeville-IIT</t>
   </si>
   <si>
@@ -512,6 +509,15 @@
   </si>
   <si>
     <t>ChIJTfF8dBOerokREI7CSi7lzZw</t>
+  </si>
+  <si>
+    <t>station name</t>
+  </si>
+  <si>
+    <t>gmaps place id</t>
+  </si>
+  <si>
+    <t>cta station id</t>
   </si>
 </sst>
 </file>
@@ -590,6 +596,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -877,2004 +887,2017 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2">
         <v>40830</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>41120</v>
-      </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>40120</v>
+        <v>41120</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>41270</v>
+        <v>40120</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>41080</v>
+        <v>41270</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>41230</v>
+        <v>41080</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
       <c r="C7">
-        <v>40130</v>
+        <v>41230</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
       <c r="C8">
-        <v>40580</v>
+        <v>40130</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
       <c r="C9">
-        <v>40910</v>
+        <v>40580</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>40990</v>
+        <v>40910</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>40240</v>
+        <v>40990</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>40240</v>
+      </c>
+      <c r="D12" t="s">
         <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>41430</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>40450</v>
+        <v>41430</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>40680</v>
+        <v>40450</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>41240</v>
+        <v>40680</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16">
-        <v>41440</v>
+        <v>41240</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17">
-        <v>41420</v>
+        <v>41440</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18">
-        <v>41200</v>
+        <v>41420</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C19">
-        <v>40660</v>
+        <v>41200</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20">
-        <v>40290</v>
+        <v>40660</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21">
-        <v>40170</v>
+        <v>40290</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22">
-        <v>41060</v>
+        <v>40170</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23">
-        <v>40010</v>
+        <v>41060</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24">
-        <v>41260</v>
+        <v>40010</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C25">
-        <v>41320</v>
+        <v>41260</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26">
-        <v>40060</v>
+        <v>41320</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C27">
-        <v>40340</v>
+        <v>40060</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C28">
-        <v>41380</v>
+        <v>40340</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29">
-        <v>40440</v>
+        <v>41380</v>
       </c>
       <c r="D29" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30">
-        <v>41360</v>
+        <v>40440</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31">
-        <v>40570</v>
+        <v>41360</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C32">
-        <v>40780</v>
+        <v>40570</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C33">
-        <v>40280</v>
+        <v>40780</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34">
-        <v>41250</v>
+        <v>40280</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C35">
-        <v>41000</v>
+        <v>41250</v>
       </c>
       <c r="D35" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C36">
-        <v>41690</v>
+        <v>41000</v>
       </c>
       <c r="D36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37">
-        <v>41410</v>
+        <v>41690</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C38">
-        <v>40710</v>
+        <v>41410</v>
       </c>
       <c r="D38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39">
-        <v>41450</v>
+        <v>40710</v>
       </c>
       <c r="D39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40">
-        <v>40420</v>
+        <v>41450</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C41">
-        <v>40970</v>
+        <v>40420</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42">
-        <v>40480</v>
+        <v>40970</v>
       </c>
       <c r="D42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43">
-        <v>40630</v>
+        <v>40480</v>
       </c>
       <c r="D43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44">
-        <v>40380</v>
+        <v>40630</v>
       </c>
       <c r="D44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C45">
-        <v>40430</v>
+        <v>40380</v>
       </c>
       <c r="D45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C46">
-        <v>41160</v>
+        <v>40430</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C47">
-        <v>41670</v>
+        <v>41160</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C48">
-        <v>40230</v>
+        <v>41670</v>
       </c>
       <c r="D48" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C49">
-        <v>40090</v>
+        <v>40230</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C50">
-        <v>40210</v>
+        <v>40090</v>
       </c>
       <c r="D50" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C51">
-        <v>40590</v>
+        <v>40210</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C52">
-        <v>40050</v>
+        <v>40590</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C53">
-        <v>40690</v>
+        <v>40050</v>
       </c>
       <c r="D53" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C54">
-        <v>40140</v>
+        <v>40690</v>
       </c>
       <c r="D54" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C55">
-        <v>40530</v>
+        <v>40140</v>
       </c>
       <c r="D55" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C56">
-        <v>40320</v>
+        <v>40530</v>
       </c>
       <c r="D56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C57">
-        <v>40720</v>
+        <v>40320</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C58">
-        <v>40390</v>
+        <v>40720</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C59">
-        <v>40520</v>
+        <v>40390</v>
       </c>
       <c r="D59" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C60">
-        <v>40870</v>
+        <v>40520</v>
       </c>
       <c r="D60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C61">
-        <v>41220</v>
+        <v>40870</v>
       </c>
       <c r="D61" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C62">
-        <v>40510</v>
+        <v>41220</v>
       </c>
       <c r="D62" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C63">
-        <v>41170</v>
+        <v>40510</v>
       </c>
       <c r="D63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C64">
-        <v>40490</v>
+        <v>41170</v>
       </c>
       <c r="D64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C65">
-        <v>40330</v>
+        <v>40490</v>
       </c>
       <c r="D65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C66">
-        <v>40760</v>
+        <v>40330</v>
       </c>
       <c r="D66" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C67">
-        <v>40940</v>
+        <v>40760</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C68">
-        <v>41130</v>
+        <v>40940</v>
       </c>
       <c r="D68" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C69">
-        <v>40980</v>
+        <v>41130</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C70">
-        <v>40020</v>
+        <v>40980</v>
       </c>
       <c r="D70" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C71">
-        <v>40750</v>
+        <v>40020</v>
       </c>
       <c r="D71" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C72">
-        <v>40850</v>
+        <v>40750</v>
       </c>
       <c r="D72" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C73">
-        <v>41490</v>
+        <v>40850</v>
       </c>
       <c r="D73" t="s">
-        <v>86</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C74">
-        <v>40900</v>
+        <v>41490</v>
       </c>
       <c r="D74" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C75">
-        <v>40810</v>
+        <v>40900</v>
       </c>
       <c r="D75" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C76">
-        <v>40300</v>
+        <v>40810</v>
       </c>
       <c r="D76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C77">
-        <v>40550</v>
+        <v>40300</v>
       </c>
       <c r="D77" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C78">
-        <v>41460</v>
+        <v>40550</v>
       </c>
       <c r="D78" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C79">
-        <v>40070</v>
+        <v>41460</v>
       </c>
       <c r="D79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C80">
-        <v>40560</v>
+        <v>40070</v>
       </c>
       <c r="D80" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C81">
-        <v>41190</v>
+        <v>40560</v>
       </c>
       <c r="D81" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C82">
-        <v>41280</v>
+        <v>41190</v>
       </c>
       <c r="D82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C83">
-        <v>41180</v>
+        <v>41280</v>
       </c>
       <c r="D83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C84">
-        <v>41040</v>
+        <v>41180</v>
       </c>
       <c r="D84" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C85">
-        <v>41070</v>
+        <v>41040</v>
       </c>
       <c r="D85" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C86">
-        <v>40250</v>
+        <v>41070</v>
       </c>
       <c r="D86" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C87">
-        <v>41150</v>
+        <v>40250</v>
       </c>
       <c r="D87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C88">
-        <v>41290</v>
+        <v>41150</v>
       </c>
       <c r="D88" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C89">
-        <v>41140</v>
+        <v>41290</v>
       </c>
       <c r="D89" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C90">
-        <v>40600</v>
+        <v>41140</v>
       </c>
       <c r="D90" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C91">
-        <v>41660</v>
+        <v>40600</v>
       </c>
       <c r="D91" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C92">
-        <v>40700</v>
+        <v>41660</v>
       </c>
       <c r="D92" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C93">
-        <v>41340</v>
+        <v>40700</v>
       </c>
       <c r="D93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C94">
-        <v>40160</v>
+        <v>41340</v>
       </c>
       <c r="D94" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C95">
-        <v>40770</v>
+        <v>40160</v>
       </c>
       <c r="D95" t="s">
-        <v>110</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C96">
-        <v>41050</v>
+        <v>40770</v>
       </c>
       <c r="D96" t="s">
-        <v>42</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C97">
-        <v>41020</v>
+        <v>41050</v>
       </c>
       <c r="D97" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C98">
-        <v>41300</v>
+        <v>41020</v>
       </c>
       <c r="D98" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C99">
-        <v>40270</v>
+        <v>41300</v>
       </c>
       <c r="D99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C100">
-        <v>40930</v>
+        <v>40270</v>
       </c>
       <c r="D100" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C101">
-        <v>40790</v>
+        <v>40930</v>
       </c>
       <c r="D101" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C102">
-        <v>41090</v>
+        <v>40790</v>
       </c>
       <c r="D102" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C103">
-        <v>41330</v>
+        <v>41090</v>
       </c>
       <c r="D103" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C104">
-        <v>41500</v>
+        <v>41330</v>
       </c>
       <c r="D104" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C105">
-        <v>41510</v>
+        <v>41500</v>
       </c>
       <c r="D105" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C106">
-        <v>40100</v>
+        <v>41510</v>
       </c>
       <c r="D106" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C107">
-        <v>40650</v>
+        <v>40100</v>
       </c>
       <c r="D107" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C108">
-        <v>40400</v>
+        <v>40650</v>
       </c>
       <c r="D108" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C109">
-        <v>40180</v>
+        <v>40400</v>
       </c>
       <c r="D109" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C110">
-        <v>41350</v>
+        <v>40180</v>
       </c>
       <c r="D110" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C111">
-        <v>41680</v>
+        <v>41350</v>
       </c>
       <c r="D111" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C112">
-        <v>40890</v>
+        <v>41680</v>
       </c>
       <c r="D112" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C113">
-        <v>41310</v>
+        <v>40890</v>
       </c>
       <c r="D113" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C114">
-        <v>41030</v>
+        <v>41310</v>
       </c>
       <c r="D114" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C115">
-        <v>40150</v>
+        <v>41030</v>
       </c>
       <c r="D115" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C116">
-        <v>40920</v>
+        <v>40150</v>
       </c>
       <c r="D116" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C117">
-        <v>40030</v>
+        <v>40920</v>
       </c>
       <c r="D117" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C118">
-        <v>40960</v>
+        <v>40030</v>
       </c>
       <c r="D118" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C119">
-        <v>40040</v>
+        <v>40960</v>
       </c>
       <c r="D119" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C120">
-        <v>40470</v>
+        <v>40040</v>
       </c>
       <c r="D120" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C121">
-        <v>40610</v>
+        <v>40470</v>
       </c>
       <c r="D121" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C122">
-        <v>41010</v>
+        <v>40610</v>
       </c>
       <c r="D122" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C123">
-        <v>41400</v>
+        <v>41010</v>
       </c>
       <c r="D123" t="s">
-        <v>139</v>
+        <v>41</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C124">
-        <v>40820</v>
+        <v>41400</v>
       </c>
       <c r="D124" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C125">
-        <v>40800</v>
+        <v>40820</v>
       </c>
       <c r="D125" t="s">
-        <v>142</v>
+        <v>32</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C126">
-        <v>40080</v>
+        <v>40800</v>
       </c>
       <c r="D126" t="s">
-        <v>3</v>
+        <v>141</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C127">
-        <v>40840</v>
+        <v>40080</v>
       </c>
       <c r="D127" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C128">
-        <v>40360</v>
+        <v>40840</v>
       </c>
       <c r="D128" t="s">
-        <v>146</v>
+        <v>41</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C129">
-        <v>40190</v>
+        <v>40360</v>
       </c>
       <c r="D129" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C130">
-        <v>40260</v>
+        <v>40190</v>
       </c>
       <c r="D130" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C131">
-        <v>40880</v>
+        <v>40260</v>
       </c>
       <c r="D131" t="s">
-        <v>150</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C132">
-        <v>40350</v>
+        <v>40880</v>
       </c>
       <c r="D132" t="s">
-        <v>3</v>
+        <v>149</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C133">
-        <v>41700</v>
+        <v>40350</v>
       </c>
       <c r="D133" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C134">
-        <v>40730</v>
+        <v>41700</v>
       </c>
       <c r="D134" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C135">
-        <v>40370</v>
+        <v>40730</v>
       </c>
       <c r="D135" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C136">
-        <v>41210</v>
+        <v>40370</v>
       </c>
       <c r="D136" t="s">
-        <v>156</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C137">
-        <v>41480</v>
+        <v>41210</v>
       </c>
       <c r="D137" t="s">
-        <v>3</v>
+        <v>155</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C138">
-        <v>40740</v>
+        <v>41480</v>
       </c>
       <c r="D138" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C139">
-        <v>40220</v>
+        <v>40740</v>
       </c>
       <c r="D139" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C140">
-        <v>40670</v>
+        <v>40220</v>
       </c>
       <c r="D140" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C141">
-        <v>40310</v>
+        <v>40670</v>
       </c>
       <c r="D141" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
+        <v>139</v>
+      </c>
+      <c r="B142" t="s">
+        <v>160</v>
+      </c>
+      <c r="C142">
+        <v>40310</v>
+      </c>
+      <c r="D142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
         <v>140</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B143" t="s">
+        <v>161</v>
+      </c>
+      <c r="C143">
+        <v>40540</v>
+      </c>
+      <c r="D143" t="s">
         <v>162</v>
-      </c>
-      <c r="C142">
-        <v>40540</v>
-      </c>
-      <c r="D142" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>